<commit_message>
Aktualisieren 4. Nov 12
</commit_message>
<xml_diff>
--- a/SUIZA.xlsx
+++ b/SUIZA.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19660" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Datum</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>92, 795, 843</t>
+  </si>
+  <si>
+    <t>GD</t>
+  </si>
+  <si>
+    <t>8, 88, 182</t>
   </si>
 </sst>
 </file>
@@ -412,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -459,6 +465,20 @@
         <v>236</v>
       </c>
     </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>41210</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>